<commit_message>
Added disclaimers and notes on data
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="854"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="854" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="22" r:id="rId1"/>
@@ -1177,7 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2843,7 +2843,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7055,8 +7055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7135,45 +7135,57 @@
         <v>4</v>
       </c>
       <c r="B2" s="14">
+        <f>0.619+((F2-0.619)/5)</f>
         <v>0.62639999999999996</v>
       </c>
       <c r="C2" s="14">
+        <f>B2+(($F2-0.619)/5)</f>
         <v>0.63379999999999992</v>
       </c>
       <c r="D2" s="14">
+        <f t="shared" ref="D2:E2" si="0">C2+(($F2-0.619)/5)</f>
         <v>0.64119999999999988</v>
       </c>
       <c r="E2" s="14">
+        <f t="shared" si="0"/>
         <v>0.64859999999999984</v>
       </c>
       <c r="F2" s="15">
         <v>0.65600000000000003</v>
       </c>
       <c r="G2" s="14">
+        <f>IF(F2="", "", F2+((K2-F2)/5))</f>
         <v>0.66380000000000006</v>
       </c>
       <c r="H2" s="14">
+        <f>IF(F2="", "", G2+((K2-F2)/5))</f>
         <v>0.67160000000000009</v>
       </c>
       <c r="I2" s="14">
+        <f>IF(F2="", "", H2+((K2-F2)/5))</f>
         <v>0.67940000000000011</v>
       </c>
       <c r="J2" s="14">
+        <f>IF(F2="", "", I2+((K2-F2)/5))</f>
         <v>0.68720000000000014</v>
       </c>
       <c r="K2" s="15">
         <v>0.69499999999999995</v>
       </c>
       <c r="L2" s="14">
+        <f t="shared" ref="L2:L8" si="1">IF(K2="", "", K2+((P2-K2)/5))</f>
         <v>0.70039999999999991</v>
       </c>
       <c r="M2" s="14">
+        <f t="shared" ref="M2:M8" si="2">IF(K2="", "", L2+((P2-K2)/5))</f>
         <v>0.70579999999999987</v>
       </c>
       <c r="N2" s="14">
+        <f t="shared" ref="N2:N8" si="3">IF(K2="", "", M2+((P2-K2)/5))</f>
         <v>0.71119999999999983</v>
       </c>
       <c r="O2" s="14">
+        <f t="shared" ref="O2:O8" si="4">IF(K2="", "", N2+((P2-K2)/5))</f>
         <v>0.71659999999999979</v>
       </c>
       <c r="P2" s="15">
@@ -7201,45 +7213,57 @@
         <v>5</v>
       </c>
       <c r="B3" s="14">
+        <f>0.605+((F3-0.605)/5)</f>
         <v>0.61360000000000003</v>
       </c>
       <c r="C3" s="14">
+        <f>B3+(($F3-0.605)/5)</f>
         <v>0.62220000000000009</v>
       </c>
       <c r="D3" s="14">
+        <f>C3+(($F3-0.605)/5)</f>
         <v>0.63080000000000014</v>
       </c>
       <c r="E3" s="14">
+        <f>D3+(($F3-0.605)/5)</f>
         <v>0.63940000000000019</v>
       </c>
       <c r="F3" s="15">
         <v>0.64800000000000002</v>
       </c>
       <c r="G3" s="14">
+        <f t="shared" ref="G3:G5" si="5">IF(F3="", "", F3+((K3-F3)/5))</f>
         <v>0.65739999999999998</v>
       </c>
       <c r="H3" s="14">
+        <f t="shared" ref="H3:H5" si="6">IF(F3="", "", G3+((K3-F3)/5))</f>
         <v>0.66679999999999995</v>
       </c>
       <c r="I3" s="14">
+        <f t="shared" ref="I3:I5" si="7">IF(F3="", "", H3+((K3-F3)/5))</f>
         <v>0.67619999999999991</v>
       </c>
       <c r="J3" s="14">
+        <f t="shared" ref="J3:J5" si="8">IF(F3="", "", I3+((K3-F3)/5))</f>
         <v>0.68559999999999988</v>
       </c>
       <c r="K3" s="15">
         <v>0.69499999999999995</v>
       </c>
       <c r="L3" s="14">
+        <f t="shared" si="1"/>
         <v>0.70019999999999993</v>
       </c>
       <c r="M3" s="14">
+        <f t="shared" si="2"/>
         <v>0.70539999999999992</v>
       </c>
       <c r="N3" s="14">
+        <f t="shared" si="3"/>
         <v>0.7105999999999999</v>
       </c>
       <c r="O3" s="14">
+        <f t="shared" si="4"/>
         <v>0.71579999999999988</v>
       </c>
       <c r="P3" s="15">
@@ -7258,7 +7282,7 @@
         <v>0.73299999999999998</v>
       </c>
       <c r="U3" s="14">
-        <f t="shared" ref="U3:U21" si="0">T3*((T3/P3)^(1/5))</f>
+        <f t="shared" ref="U3:U21" si="9">T3*((T3/P3)^(1/5))</f>
         <v>0.73542386113124025</v>
       </c>
     </row>
@@ -7267,45 +7291,57 @@
         <v>6</v>
       </c>
       <c r="B4" s="14">
+        <f>0.609+((F4-0.609)/5)</f>
         <v>0.61519999999999997</v>
       </c>
       <c r="C4" s="14">
+        <f>B4+(($F4-0.609)/5)</f>
         <v>0.62139999999999995</v>
       </c>
       <c r="D4" s="14">
+        <f t="shared" ref="D4:E4" si="10">C4+(($F4-0.609)/5)</f>
         <v>0.62759999999999994</v>
       </c>
       <c r="E4" s="14">
+        <f t="shared" si="10"/>
         <v>0.63379999999999992</v>
       </c>
       <c r="F4" s="15">
         <v>0.64</v>
       </c>
       <c r="G4" s="14">
+        <f t="shared" si="5"/>
         <v>0.64959999999999996</v>
       </c>
       <c r="H4" s="14">
+        <f t="shared" si="6"/>
         <v>0.6591999999999999</v>
       </c>
       <c r="I4" s="14">
+        <f t="shared" si="7"/>
         <v>0.66879999999999984</v>
       </c>
       <c r="J4" s="14">
+        <f t="shared" si="8"/>
         <v>0.67839999999999978</v>
       </c>
       <c r="K4" s="15">
         <v>0.68799999999999994</v>
       </c>
       <c r="L4" s="14">
+        <f t="shared" si="1"/>
         <v>0.6986</v>
       </c>
       <c r="M4" s="14">
+        <f t="shared" si="2"/>
         <v>0.70920000000000005</v>
       </c>
       <c r="N4" s="14">
+        <f t="shared" si="3"/>
         <v>0.71980000000000011</v>
       </c>
       <c r="O4" s="14">
+        <f t="shared" si="4"/>
         <v>0.73040000000000016</v>
       </c>
       <c r="P4" s="15">
@@ -7324,7 +7360,7 @@
         <v>0.751</v>
       </c>
       <c r="U4" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.75301613640405651</v>
       </c>
     </row>
@@ -7348,30 +7384,38 @@
         <v>0.68300000000000005</v>
       </c>
       <c r="G5" s="14">
+        <f t="shared" si="5"/>
         <v>0.69100000000000006</v>
       </c>
       <c r="H5" s="14">
+        <f t="shared" si="6"/>
         <v>0.69900000000000007</v>
       </c>
       <c r="I5" s="14">
+        <f t="shared" si="7"/>
         <v>0.70700000000000007</v>
       </c>
       <c r="J5" s="14">
+        <f t="shared" si="8"/>
         <v>0.71500000000000008</v>
       </c>
       <c r="K5" s="15">
         <v>0.72299999999999998</v>
       </c>
       <c r="L5" s="14">
+        <f t="shared" si="1"/>
         <v>0.73560000000000003</v>
       </c>
       <c r="M5" s="14">
+        <f t="shared" si="2"/>
         <v>0.74820000000000009</v>
       </c>
       <c r="N5" s="14">
+        <f t="shared" si="3"/>
         <v>0.76080000000000014</v>
       </c>
       <c r="O5" s="14">
+        <f t="shared" si="4"/>
         <v>0.7734000000000002</v>
       </c>
       <c r="P5" s="15">
@@ -7390,7 +7434,7 @@
         <v>0.79800000000000004</v>
       </c>
       <c r="U5" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.80042189583726564</v>
       </c>
     </row>
@@ -7427,15 +7471,19 @@
         <v>0.69699999999999995</v>
       </c>
       <c r="L6" s="14">
+        <f t="shared" si="1"/>
         <v>0.6996</v>
       </c>
       <c r="M6" s="14">
+        <f t="shared" si="2"/>
         <v>0.70220000000000005</v>
       </c>
       <c r="N6" s="14">
+        <f t="shared" si="3"/>
         <v>0.70480000000000009</v>
       </c>
       <c r="O6" s="14">
+        <f t="shared" si="4"/>
         <v>0.70740000000000014</v>
       </c>
       <c r="P6" s="15">
@@ -7454,7 +7502,7 @@
         <v>0.73299999999999998</v>
       </c>
       <c r="U6" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.73768864715483828</v>
       </c>
     </row>
@@ -7478,30 +7526,38 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="G7" s="14">
+        <f t="shared" ref="G7:G8" si="11">IF(F7="", "", F7+((K7-F7)/5))</f>
         <v>0.67980000000000007</v>
       </c>
       <c r="H7" s="14">
+        <f t="shared" ref="H7:H8" si="12">IF(F7="", "", G7+((K7-F7)/5))</f>
         <v>0.6876000000000001</v>
       </c>
       <c r="I7" s="14">
+        <f t="shared" ref="I7:I8" si="13">IF(F7="", "", H7+((K7-F7)/5))</f>
         <v>0.69540000000000013</v>
       </c>
       <c r="J7" s="14">
+        <f t="shared" ref="J7:J8" si="14">IF(F7="", "", I7+((K7-F7)/5))</f>
         <v>0.70320000000000016</v>
       </c>
       <c r="K7" s="15">
         <v>0.71099999999999997</v>
       </c>
       <c r="L7" s="14">
+        <f t="shared" si="1"/>
         <v>0.71579999999999999</v>
       </c>
       <c r="M7" s="14">
+        <f t="shared" si="2"/>
         <v>0.72060000000000002</v>
       </c>
       <c r="N7" s="14">
+        <f t="shared" si="3"/>
         <v>0.72540000000000004</v>
       </c>
       <c r="O7" s="14">
+        <f t="shared" si="4"/>
         <v>0.73020000000000007</v>
       </c>
       <c r="P7" s="15">
@@ -7520,7 +7576,7 @@
         <v>0.754</v>
       </c>
       <c r="U7" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.75785853714445162</v>
       </c>
     </row>
@@ -7529,45 +7585,57 @@
         <v>9</v>
       </c>
       <c r="B8" s="14">
+        <f>0.664+((F8-0.664)/5)</f>
         <v>0.66700000000000004</v>
       </c>
       <c r="C8" s="14">
+        <f>B8+(($F8-0.664)/5)</f>
         <v>0.67</v>
       </c>
       <c r="D8" s="14">
+        <f t="shared" ref="D8:E8" si="15">C8+(($F8-0.664)/5)</f>
         <v>0.67300000000000004</v>
       </c>
       <c r="E8" s="14">
+        <f t="shared" si="15"/>
         <v>0.67600000000000005</v>
       </c>
       <c r="F8" s="15">
         <v>0.67900000000000005</v>
       </c>
       <c r="G8" s="14">
+        <f t="shared" si="11"/>
         <v>0.69240000000000002</v>
       </c>
       <c r="H8" s="14">
+        <f t="shared" si="12"/>
         <v>0.70579999999999998</v>
       </c>
       <c r="I8" s="14">
+        <f t="shared" si="13"/>
         <v>0.71919999999999995</v>
       </c>
       <c r="J8" s="14">
+        <f t="shared" si="14"/>
         <v>0.73259999999999992</v>
       </c>
       <c r="K8" s="15">
         <v>0.746</v>
       </c>
       <c r="L8" s="14">
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="M8" s="14">
+        <f t="shared" si="2"/>
         <v>0.754</v>
       </c>
       <c r="N8" s="14">
+        <f t="shared" si="3"/>
         <v>0.75800000000000001</v>
       </c>
       <c r="O8" s="14">
+        <f t="shared" si="4"/>
         <v>0.76200000000000001</v>
       </c>
       <c r="P8" s="15">
@@ -7586,7 +7654,7 @@
         <v>0.78800000000000003</v>
       </c>
       <c r="U8" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.79247524912945666</v>
       </c>
     </row>
@@ -7644,45 +7712,57 @@
         <v>21</v>
       </c>
       <c r="B10" s="14">
+        <f>0.562+((F10-0.562)/5)</f>
         <v>0.56820000000000004</v>
       </c>
       <c r="C10" s="14">
+        <f>B10+(($F10-0.562)/5)</f>
         <v>0.57440000000000002</v>
       </c>
       <c r="D10" s="14">
+        <f t="shared" ref="D10:E10" si="16">C10+(($F10-0.562)/5)</f>
         <v>0.5806</v>
       </c>
       <c r="E10" s="14">
+        <f t="shared" si="16"/>
         <v>0.58679999999999999</v>
       </c>
       <c r="F10" s="15">
         <v>0.59299999999999997</v>
       </c>
       <c r="G10" s="14">
+        <f>IF(F10="", "", F10+((K10-F10)/5))</f>
         <v>0.59719999999999995</v>
       </c>
       <c r="H10" s="14">
+        <f>IF(F10="", "", G10+((K10-F10)/5))</f>
         <v>0.60139999999999993</v>
       </c>
       <c r="I10" s="14">
+        <f>IF(F10="", "", H10+((K10-F10)/5))</f>
         <v>0.60559999999999992</v>
       </c>
       <c r="J10" s="14">
+        <f>IF(F10="", "", I10+((K10-F10)/5))</f>
         <v>0.6097999999999999</v>
       </c>
       <c r="K10" s="15">
         <v>0.61399999999999999</v>
       </c>
       <c r="L10" s="14">
+        <f t="shared" ref="L10:L16" si="17">IF(K10="", "", K10+((P10-K10)/5))</f>
         <v>0.61799999999999999</v>
       </c>
       <c r="M10" s="14">
+        <f t="shared" ref="M10:M16" si="18">IF(K10="", "", L10+((P10-K10)/5))</f>
         <v>0.622</v>
       </c>
       <c r="N10" s="14">
+        <f t="shared" ref="N10:N16" si="19">IF(K10="", "", M10+((P10-K10)/5))</f>
         <v>0.626</v>
       </c>
       <c r="O10" s="14">
+        <f t="shared" ref="O10:O16" si="20">IF(K10="", "", N10+((P10-K10)/5))</f>
         <v>0.63</v>
       </c>
       <c r="P10" s="15">
@@ -7701,7 +7781,7 @@
         <v>0.65500000000000003</v>
       </c>
       <c r="U10" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.65928274354650751</v>
       </c>
     </row>
@@ -7738,15 +7818,19 @@
         <v>0.69699999999999995</v>
       </c>
       <c r="L11" s="14">
+        <f t="shared" si="17"/>
         <v>0.70519999999999994</v>
       </c>
       <c r="M11" s="14">
+        <f t="shared" si="18"/>
         <v>0.71339999999999992</v>
       </c>
       <c r="N11" s="14">
+        <f t="shared" si="19"/>
         <v>0.72159999999999991</v>
       </c>
       <c r="O11" s="14">
+        <f t="shared" si="20"/>
         <v>0.72979999999999989</v>
       </c>
       <c r="P11" s="15">
@@ -7765,7 +7849,7 @@
         <v>0.747</v>
       </c>
       <c r="U11" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.7488131281335183</v>
       </c>
     </row>
@@ -7774,45 +7858,57 @@
         <v>12</v>
       </c>
       <c r="B12" s="14">
+        <f>0.594+((F12-0.594)/5)</f>
         <v>0.59460000000000002</v>
       </c>
       <c r="C12" s="14">
+        <f>B12+(($F12-0.594)/5)</f>
         <v>0.59520000000000006</v>
       </c>
       <c r="D12" s="14">
+        <f t="shared" ref="D12:E12" si="21">C12+(($F12-0.594)/5)</f>
         <v>0.59580000000000011</v>
       </c>
       <c r="E12" s="14">
+        <f t="shared" si="21"/>
         <v>0.59640000000000015</v>
       </c>
       <c r="F12" s="15">
         <v>0.59699999999999998</v>
       </c>
       <c r="G12" s="14">
+        <f>IF(F12="", "", F12+((K12-F12)/5))</f>
         <v>0.60739999999999994</v>
       </c>
       <c r="H12" s="14">
+        <f>IF(F12="", "", G12+((K12-F12)/5))</f>
         <v>0.6177999999999999</v>
       </c>
       <c r="I12" s="14">
+        <f>IF(F12="", "", H12+((K12-F12)/5))</f>
         <v>0.62819999999999987</v>
       </c>
       <c r="J12" s="14">
+        <f>IF(F12="", "", I12+((K12-F12)/5))</f>
         <v>0.63859999999999983</v>
       </c>
       <c r="K12" s="15">
         <v>0.64900000000000002</v>
       </c>
       <c r="L12" s="14">
+        <f t="shared" si="17"/>
         <v>0.65360000000000007</v>
       </c>
       <c r="M12" s="14">
+        <f t="shared" si="18"/>
         <v>0.65820000000000012</v>
       </c>
       <c r="N12" s="14">
+        <f t="shared" si="19"/>
         <v>0.66280000000000017</v>
       </c>
       <c r="O12" s="14">
+        <f t="shared" si="20"/>
         <v>0.66740000000000022</v>
       </c>
       <c r="P12" s="15">
@@ -7831,7 +7927,7 @@
         <v>0.69299999999999995</v>
       </c>
       <c r="U12" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.69727810282014591</v>
       </c>
     </row>
@@ -7868,15 +7964,19 @@
         <v>0.75</v>
       </c>
       <c r="L13" s="14">
+        <f t="shared" si="17"/>
         <v>0.75839999999999996</v>
       </c>
       <c r="M13" s="14">
+        <f t="shared" si="18"/>
         <v>0.76679999999999993</v>
       </c>
       <c r="N13" s="14">
+        <f t="shared" si="19"/>
         <v>0.77519999999999989</v>
       </c>
       <c r="O13" s="14">
+        <f t="shared" si="20"/>
         <v>0.78359999999999985</v>
       </c>
       <c r="P13" s="15">
@@ -7895,7 +7995,7 @@
         <v>0.80200000000000005</v>
       </c>
       <c r="U13" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.80401510078777483</v>
       </c>
     </row>
@@ -7904,45 +8004,57 @@
         <v>14</v>
       </c>
       <c r="B14" s="14">
+        <f>0.694+((F14-0.694)/5)</f>
         <v>0.69719999999999993</v>
       </c>
       <c r="C14" s="14">
+        <f>B14+(($F14-0.694)/5)</f>
         <v>0.70039999999999991</v>
       </c>
       <c r="D14" s="14">
+        <f t="shared" ref="D14:E14" si="22">C14+(($F14-0.694)/5)</f>
         <v>0.70359999999999989</v>
       </c>
       <c r="E14" s="14">
+        <f t="shared" si="22"/>
         <v>0.70679999999999987</v>
       </c>
       <c r="F14" s="15">
         <v>0.71</v>
       </c>
       <c r="G14" s="14">
+        <f t="shared" ref="G14:G16" si="23">IF(F14="", "", F14+((K14-F14)/5))</f>
         <v>0.71619999999999995</v>
       </c>
       <c r="H14" s="14">
+        <f t="shared" ref="H14:H16" si="24">IF(F14="", "", G14+((K14-F14)/5))</f>
         <v>0.72239999999999993</v>
       </c>
       <c r="I14" s="14">
+        <f t="shared" ref="I14:I16" si="25">IF(F14="", "", H14+((K14-F14)/5))</f>
         <v>0.72859999999999991</v>
       </c>
       <c r="J14" s="14">
+        <f t="shared" ref="J14:J16" si="26">IF(F14="", "", I14+((K14-F14)/5))</f>
         <v>0.7347999999999999</v>
       </c>
       <c r="K14" s="15">
         <v>0.74099999999999999</v>
       </c>
       <c r="L14" s="14">
+        <f t="shared" si="17"/>
         <v>0.74419999999999997</v>
       </c>
       <c r="M14" s="14">
+        <f t="shared" si="18"/>
         <v>0.74739999999999995</v>
       </c>
       <c r="N14" s="14">
+        <f t="shared" si="19"/>
         <v>0.75059999999999993</v>
       </c>
       <c r="O14" s="14">
+        <f t="shared" si="20"/>
         <v>0.75379999999999991</v>
       </c>
       <c r="P14" s="15">
@@ -7961,7 +8073,7 @@
         <v>0.77100000000000002</v>
       </c>
       <c r="U14" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.77383091804590176</v>
       </c>
     </row>
@@ -7970,45 +8082,57 @@
         <v>15</v>
       </c>
       <c r="B15" s="14">
+        <f>0.539+((F15-0.539)/5)</f>
         <v>0.53820000000000001</v>
       </c>
       <c r="C15" s="14">
+        <f>B15+(($F15-0.539)/5)</f>
         <v>0.53739999999999999</v>
       </c>
       <c r="D15" s="14">
+        <f t="shared" ref="D15:E15" si="27">C15+(($F15-0.539)/5)</f>
         <v>0.53659999999999997</v>
       </c>
       <c r="E15" s="14">
+        <f t="shared" si="27"/>
         <v>0.53579999999999994</v>
       </c>
       <c r="F15" s="15">
         <v>0.53500000000000003</v>
       </c>
       <c r="G15" s="14">
+        <f t="shared" si="23"/>
         <v>0.54380000000000006</v>
       </c>
       <c r="H15" s="14">
+        <f t="shared" si="24"/>
         <v>0.55260000000000009</v>
       </c>
       <c r="I15" s="14">
+        <f t="shared" si="25"/>
         <v>0.56140000000000012</v>
       </c>
       <c r="J15" s="14">
+        <f t="shared" si="26"/>
         <v>0.57020000000000015</v>
       </c>
       <c r="K15" s="15">
         <v>0.57899999999999996</v>
       </c>
       <c r="L15" s="14">
+        <f t="shared" si="17"/>
         <v>0.58479999999999999</v>
       </c>
       <c r="M15" s="14">
+        <f t="shared" si="18"/>
         <v>0.59060000000000001</v>
       </c>
       <c r="N15" s="14">
+        <f t="shared" si="19"/>
         <v>0.59640000000000004</v>
       </c>
       <c r="O15" s="14">
+        <f t="shared" si="20"/>
         <v>0.60220000000000007</v>
       </c>
       <c r="P15" s="15">
@@ -8027,7 +8151,7 @@
         <v>0.624</v>
       </c>
       <c r="U15" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.62725017588315013</v>
       </c>
     </row>
@@ -8036,45 +8160,57 @@
         <v>16</v>
       </c>
       <c r="B16" s="14">
+        <f>0.604+((F16-0.604)/5)</f>
         <v>0.61380000000000001</v>
       </c>
       <c r="C16" s="14">
+        <f>B16+(($F16-0.604)/5)</f>
         <v>0.62360000000000004</v>
       </c>
       <c r="D16" s="14">
+        <f t="shared" ref="D16:E16" si="28">C16+(($F16-0.604)/5)</f>
         <v>0.63340000000000007</v>
       </c>
       <c r="E16" s="14">
+        <f t="shared" si="28"/>
         <v>0.6432000000000001</v>
       </c>
       <c r="F16" s="15">
         <v>0.65300000000000002</v>
       </c>
       <c r="G16" s="14">
+        <f t="shared" si="23"/>
         <v>0.65980000000000005</v>
       </c>
       <c r="H16" s="14">
+        <f t="shared" si="24"/>
         <v>0.66660000000000008</v>
       </c>
       <c r="I16" s="14">
+        <f t="shared" si="25"/>
         <v>0.67340000000000011</v>
       </c>
       <c r="J16" s="14">
+        <f t="shared" si="26"/>
         <v>0.68020000000000014</v>
       </c>
       <c r="K16" s="15">
         <v>0.68700000000000006</v>
       </c>
       <c r="L16" s="14">
+        <f t="shared" si="17"/>
         <v>0.69720000000000004</v>
       </c>
       <c r="M16" s="14">
+        <f t="shared" si="18"/>
         <v>0.70740000000000003</v>
       </c>
       <c r="N16" s="14">
+        <f t="shared" si="19"/>
         <v>0.71760000000000002</v>
       </c>
       <c r="O16" s="14">
+        <f t="shared" si="20"/>
         <v>0.7278</v>
       </c>
       <c r="P16" s="15">
@@ -8093,7 +8229,7 @@
         <v>0.76100000000000001</v>
       </c>
       <c r="U16" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.76568531125442929</v>
       </c>
     </row>
@@ -8155,7 +8291,7 @@
         <v>0.68799999999999994</v>
       </c>
       <c r="U17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.69248645022774258</v>
       </c>
     </row>
@@ -8164,45 +8300,57 @@
         <v>18</v>
       </c>
       <c r="B18" s="14">
+        <f>0.662+((F18-0.662)/5)</f>
         <v>0.66320000000000001</v>
       </c>
       <c r="C18" s="14">
+        <f>B18+(($F18-0.662)/5)</f>
         <v>0.66439999999999999</v>
       </c>
       <c r="D18" s="14">
+        <f t="shared" ref="D18:E18" si="29">C18+(($F18-0.662)/5)</f>
         <v>0.66559999999999997</v>
       </c>
       <c r="E18" s="14">
+        <f t="shared" si="29"/>
         <v>0.66679999999999995</v>
       </c>
       <c r="F18" s="15">
         <v>0.66800000000000004</v>
       </c>
       <c r="G18" s="14">
+        <f t="shared" ref="G18:G21" si="30">IF(F18="", "", F18+((K18-F18)/5))</f>
         <v>0.67700000000000005</v>
       </c>
       <c r="H18" s="14">
+        <f t="shared" ref="H18:H21" si="31">IF(F18="", "", G18+((K18-F18)/5))</f>
         <v>0.68600000000000005</v>
       </c>
       <c r="I18" s="14">
+        <f t="shared" ref="I18:I21" si="32">IF(F18="", "", H18+((K18-F18)/5))</f>
         <v>0.69500000000000006</v>
       </c>
       <c r="J18" s="14">
+        <f t="shared" ref="J18:J21" si="33">IF(F18="", "", I18+((K18-F18)/5))</f>
         <v>0.70400000000000007</v>
       </c>
       <c r="K18" s="15">
         <v>0.71299999999999997</v>
       </c>
       <c r="L18" s="14">
+        <f t="shared" ref="L18:L21" si="34">IF(K18="", "", K18+((P18-K18)/5))</f>
         <v>0.71679999999999999</v>
       </c>
       <c r="M18" s="14">
+        <f t="shared" ref="M18:M21" si="35">IF(K18="", "", L18+((P18-K18)/5))</f>
         <v>0.72060000000000002</v>
       </c>
       <c r="N18" s="14">
+        <f t="shared" ref="N18:N21" si="36">IF(K18="", "", M18+((P18-K18)/5))</f>
         <v>0.72440000000000004</v>
       </c>
       <c r="O18" s="14">
+        <f t="shared" ref="O18:O21" si="37">IF(K18="", "", N18+((P18-K18)/5))</f>
         <v>0.72820000000000007</v>
       </c>
       <c r="P18" s="15">
@@ -8221,7 +8369,7 @@
         <v>0.747</v>
       </c>
       <c r="U18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.75003668552476099</v>
       </c>
     </row>
@@ -8245,30 +8393,38 @@
         <v>0.59399999999999997</v>
       </c>
       <c r="G19" s="14">
+        <f t="shared" si="30"/>
         <v>0.60019999999999996</v>
       </c>
       <c r="H19" s="14">
+        <f t="shared" si="31"/>
         <v>0.60639999999999994</v>
       </c>
       <c r="I19" s="14">
+        <f t="shared" si="32"/>
         <v>0.61259999999999992</v>
       </c>
       <c r="J19" s="14">
+        <f t="shared" si="33"/>
         <v>0.61879999999999991</v>
       </c>
       <c r="K19" s="15">
         <v>0.625</v>
       </c>
       <c r="L19" s="14">
+        <f t="shared" si="34"/>
         <v>0.63100000000000001</v>
       </c>
       <c r="M19" s="14">
+        <f t="shared" si="35"/>
         <v>0.63700000000000001</v>
       </c>
       <c r="N19" s="14">
+        <f t="shared" si="36"/>
         <v>0.64300000000000002</v>
       </c>
       <c r="O19" s="14">
+        <f t="shared" si="37"/>
         <v>0.64900000000000002</v>
       </c>
       <c r="P19" s="15">
@@ -8287,7 +8443,7 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="U19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.67907269380234025</v>
       </c>
     </row>
@@ -8295,47 +8451,59 @@
       <c r="A20" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="17">
-        <v>0.61973999999999996</v>
-      </c>
-      <c r="C20" s="17">
-        <v>0.62427999999999995</v>
-      </c>
-      <c r="D20" s="17">
-        <v>0.62881999999999993</v>
-      </c>
-      <c r="E20" s="17">
-        <v>0.63336000000000003</v>
+      <c r="B20" s="14">
+        <f>0.6152+((F20-0.6152)/5)</f>
+        <v>0.62028307692307694</v>
+      </c>
+      <c r="C20" s="14">
+        <f>B20+(($F20-0.6152)/5)</f>
+        <v>0.6253661538461539</v>
+      </c>
+      <c r="D20" s="14">
+        <f t="shared" ref="D20:E20" si="38">C20+(($F20-0.6152)/5)</f>
+        <v>0.63044923076923087</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="38"/>
+        <v>0.63553230769230784</v>
       </c>
       <c r="F20" s="18">
         <v>0.64061538461538459</v>
       </c>
-      <c r="G20" s="17">
-        <v>0.64889230769230766</v>
-      </c>
-      <c r="H20" s="17">
-        <v>0.65716923076923073</v>
-      </c>
-      <c r="I20" s="17">
-        <v>0.66544615384615391</v>
-      </c>
-      <c r="J20" s="17">
-        <v>0.67372307692307687</v>
+      <c r="G20" s="14">
+        <f t="shared" si="30"/>
+        <v>0.65011730769230769</v>
+      </c>
+      <c r="H20" s="14">
+        <f t="shared" si="31"/>
+        <v>0.65961923076923079</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="32"/>
+        <v>0.66912115384615389</v>
+      </c>
+      <c r="J20" s="14">
+        <f t="shared" si="33"/>
+        <v>0.678623076923077</v>
       </c>
       <c r="K20" s="18">
         <v>0.68812499999999999</v>
       </c>
-      <c r="L20" s="17">
-        <v>0.69433749999999994</v>
-      </c>
-      <c r="M20" s="17">
-        <v>0.70055000000000001</v>
-      </c>
-      <c r="N20" s="17">
-        <v>0.70676249999999996</v>
-      </c>
-      <c r="O20" s="17">
-        <v>0.71297499999999991</v>
+      <c r="L20" s="14">
+        <f t="shared" si="34"/>
+        <v>0.69371176470588236</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="35"/>
+        <v>0.69929852941176474</v>
+      </c>
+      <c r="N20" s="14">
+        <f t="shared" si="36"/>
+        <v>0.70488529411764711</v>
+      </c>
+      <c r="O20" s="14">
+        <f t="shared" si="37"/>
+        <v>0.71047205882352948</v>
       </c>
       <c r="P20" s="18">
         <v>0.71605882352941175</v>
@@ -8353,7 +8521,7 @@
         <v>0.7325294117647061</v>
       </c>
       <c r="U20" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.7358687156387469</v>
       </c>
     </row>
@@ -8361,47 +8529,59 @@
       <c r="A21" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="17">
-        <v>0.78350000000000009</v>
-      </c>
-      <c r="C21" s="17">
-        <v>0.79010714285714279</v>
-      </c>
-      <c r="D21" s="17">
-        <v>0.79671428571428571</v>
-      </c>
-      <c r="E21" s="17">
-        <v>0.80332142857142852</v>
+      <c r="B21" s="14">
+        <f>0.776892857142857+((F21-0.776892857142857)/5)</f>
+        <v>0.78349999999999997</v>
+      </c>
+      <c r="C21" s="14">
+        <f>B21+(($F21-0.776892857142857)/5)</f>
+        <v>0.7901071428571429</v>
+      </c>
+      <c r="D21" s="14">
+        <f t="shared" ref="D21:E21" si="39">C21+(($F21-0.776892857142857)/5)</f>
+        <v>0.79671428571428582</v>
+      </c>
+      <c r="E21" s="14">
+        <f t="shared" si="39"/>
+        <v>0.80332142857142874</v>
       </c>
       <c r="F21" s="18">
         <v>0.80992857142857144</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="14">
+        <f t="shared" si="30"/>
         <v>0.81574285714285721</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="14">
+        <f t="shared" si="31"/>
         <v>0.82155714285714299</v>
       </c>
-      <c r="I21" s="17">
-        <v>0.82737142857142854</v>
-      </c>
-      <c r="J21" s="17">
-        <v>0.83318571428571442</v>
+      <c r="I21" s="14">
+        <f t="shared" si="32"/>
+        <v>0.82737142857142876</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="33"/>
+        <v>0.83318571428571453</v>
       </c>
       <c r="K21" s="18">
         <v>0.83900000000000008</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="14">
+        <f t="shared" si="34"/>
         <v>0.84260000000000002</v>
       </c>
-      <c r="M21" s="17">
-        <v>0.84620000000000017</v>
-      </c>
-      <c r="N21" s="17">
-        <v>0.84980000000000022</v>
-      </c>
-      <c r="O21" s="17">
-        <v>0.85340000000000027</v>
+      <c r="M21" s="14">
+        <f t="shared" si="35"/>
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="36"/>
+        <v>0.84979999999999989</v>
+      </c>
+      <c r="O21" s="14">
+        <f t="shared" si="37"/>
+        <v>0.85339999999999983</v>
       </c>
       <c r="P21" s="18">
         <v>0.85699999999999998</v>
@@ -8419,7 +8599,7 @@
         <v>0.86567857142857141</v>
       </c>
       <c r="U21" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0.86742480358577945</v>
       </c>
     </row>
@@ -11244,7 +11424,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>